<commit_message>
Added a "MikeSuggestedFormat" tab
The new tab shows a somewhat different approach to writing a testplan.  The goals of this approach are to make the feature being tested more obvious to the reader and to be explicit about the verification coverage goals for each feature.
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bit manipulation" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MikeSuggestedFormat" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t xml:space="preserve">Requirement reference</t>
   </si>
@@ -37,7 +38,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Pass/Fail Critiera</t>
+    <t xml:space="preserve">Pass/Fail Criteria</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -187,6 +188,89 @@
   </si>
   <si>
     <t xml:space="preserve">Rotation to the right or rs1 by M (rs2) positions is correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.3.1 Bit Manipulation Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.extract instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extract ls3 bits from rs1, starting from position ls2.  32-bit sign extend the result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover all extracted bit-widths 0..32
+Cover all bit starting positions 0..31
+Cover both negative and positive values of extracted data
+Cover case when ls3+ls2==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All bit extractions performed as expected.
+Q: what happens when ls3+l2&gt;32?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compliance
+Random Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not yet coded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.extractu instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extract ls3 bits from rs1, starting from position ls2.  32-bit zero extend the result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.extractr instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit sign extend the result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover all extracted bit-widths 0..32
+Cover all bit starting positions 0..31
+Cover both negative and positive values of extracted data
+Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.extractur instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit zero extend the result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.insert instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.insertr instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.bclr instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.bclrr instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.bset instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.bsetr instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.ff1 instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.fl1 instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.clb instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.cnt instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.ror instruction</t>
   </si>
 </sst>
 </file>
@@ -270,21 +354,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -367,232 +467,232 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="57.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="9" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="57.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="9" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" customFormat="false" ht="119" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="5" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="6" customFormat="false" ht="83" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="7" customFormat="false" ht="83" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="8" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="10" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1048576" s="3" t="s">
+    <row r="1048576" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1048576" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -605,4 +705,345 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="57.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="9" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="1" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rD and rs1 should be all possible GPRs.
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -199,7 +199,8 @@
     <t xml:space="preserve"> Extract ls3 bits from rs1, starting from position ls2.  32-bit sign extend the result.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cover all extracted bit-widths 0..32
+    <t xml:space="preserve">rD and rs1 should be all possible GPRs.
+Cover all extracted bit-widths 0..32
 Cover all bit starting positions 0..31
 Cover both negative and positive values of extracted data
 Cover case when ls3+ls2==32 and &gt; 32</t>
@@ -228,7 +229,8 @@
     <t xml:space="preserve"> Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit sign extend the result.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cover all extracted bit-widths 0..32
+    <t xml:space="preserve">rD and rs1 should be all possible GPRs.
+Cover all extracted bit-widths 0..32
 Cover all bit starting positions 0..31
 Cover both negative and positive values of extracted data
 Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32</t>
@@ -715,7 +717,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -784,7 +786,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -810,7 +812,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -836,7 +838,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update test plans: xpulp-general-alu and xpulp-bitmanipulations
Signed-off-by: alfredoh1234 <alfredo.herrera@ieee.org>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aherrera\Documents\4_OSHW_Design&amp;Verif_40%\core-v-docs\verif\CV32E40P\VerificationPlan\xpulp_instruction_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1C8671-783E-4E44-9C46-AF8E5F0F02E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C4E8D-3759-459F-A1D5-4486AA2C2A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17360" yWindow="-50" windowWidth="21060" windowHeight="20970" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="38460" yWindow="80" windowWidth="23380" windowHeight="21020" xr2:uid="{9416510B-1E66-491B-BB72-4AAF856B4E22}"/>
+    <workbookView xWindow="38450" yWindow="8650" windowWidth="38060" windowHeight="12540" xr2:uid="{9416510B-1E66-491B-BB72-4AAF856B4E22}"/>
   </bookViews>
   <sheets>
     <sheet name="bit-manipulation" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -276,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -299,142 +298,211 @@
     <t>Coverage Method</t>
   </si>
   <si>
-    <t>p.extract instruction</t>
-  </si>
-  <si>
-    <t>rD and rs1 should be all possible GPRs.
+    <t>Not yet coded</t>
+  </si>
+  <si>
+    <t>RI5CY: User Manual
+Dec. 2019 Revision 4.2 14.3.1</t>
+  </si>
+  <si>
+    <t>Sub-Feature</t>
+  </si>
+  <si>
+    <t>Feature Description</t>
+  </si>
+  <si>
+    <t>Clear ls3 bits in rD starting from position ls2. No zero or sign extension</t>
+  </si>
+  <si>
+    <t>Set ls3 bits in rD starting from position ls2. No zero or sign extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find first "1" bit in rs1, starting from LSB, and write position in rD.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find last "1" bit in rs1, starting from MSB, and write position in rD.  </t>
+  </si>
+  <si>
+    <t>Count the number of consecutive 1’s or 0’s in rs1 starting from MSB.</t>
+  </si>
+  <si>
+    <t>Count the total number of 1’s in rs1.</t>
+  </si>
+  <si>
+    <t>Rotate right rs1 by rs2 number of bits</t>
+  </si>
+  <si>
+    <t>XPULP Bit Manipulation</t>
+  </si>
+  <si>
+    <t>p.extract rD, rs1, Is3, Is2</t>
+  </si>
+  <si>
+    <t>p.extractu rD, rs1, Is3, Is2</t>
+  </si>
+  <si>
+    <t>p.extractr rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>p.extractur rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>p.insert rD, rs1, Is3, Is2</t>
+  </si>
+  <si>
+    <t>p.insertr rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>p.bclr rD, rs1, Is3, Is2</t>
+  </si>
+  <si>
+    <t>p.bset rD, rs1, Is3, Is2</t>
+  </si>
+  <si>
+    <t>p.bclrr rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>p.bsetr rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>p.ff1 rD, rs1</t>
+  </si>
+  <si>
+    <t>p.fl1 rD, rs1</t>
+  </si>
+  <si>
+    <t>p.clb rD, rs1</t>
+  </si>
+  <si>
+    <t>p.cnt rD, rs1</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
 Cover all extracted bit-widths 0..32
 Cover all bit starting positions 0..31
-Cover both negative and positive values of extracted data
 Cover case when ls3+ls2==32 and &gt; 32</t>
   </si>
   <si>
-    <t>Compliance
-Random Instructions</t>
-  </si>
-  <si>
-    <t>Not yet coded</t>
-  </si>
-  <si>
-    <t>p.extractu instruction</t>
-  </si>
-  <si>
-    <t>p.extractr instruction</t>
-  </si>
-  <si>
-    <t>rD and rs1 should be all possible GPRs.
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs)..
 Cover all extracted bit-widths 0..32
 Cover all bit starting positions 0..31
-Cover both negative and positive values of extracted data
+ Cover case when ls3+ls2==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t>Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit zero extend over ls2-th bit in the result.</t>
+  </si>
+  <si>
+    <t>Extract ls3 bits from rs1, starting from position ls2.  32-bit sign extend over ls2-th bit in the result.</t>
+  </si>
+  <si>
+    <t>Extract ls3 bits from rs1, starting from position ls2.  32-bit zero extend over ls2-th bit in the result.</t>
+  </si>
+  <si>
+    <t>Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit sign extend over ls2-th bit in the result.</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all bit-widths to be inserted 0..32
+Cover all bit starting positions 0..31
+Cover case when ls3+ls2==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert rs1[ls3:0] into rD starting from position ls2. No zero or sign extension. </t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all bit-widths to be cleared 0..32
+Cover all bit starting positions 0..31
+Cover case when ls3+ls2==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t>Insert rs1[rs2[9:5]] into rD starting from position rs2[4:0]. No zero or sign extension</t>
+  </si>
+  <si>
+    <t>Clear rs1[rs2[9:5]] bits in rD starting from position rs2[4:0]. No zero or sign extension</t>
+  </si>
+  <si>
+    <t>Set rs1[rs2[9:5]] bits in rD starting from position rs2[4:0]. No zero or sign extension</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all bit-widths to be set 0..32
+Cover all bit starting positions 0..31
+Cover case when ls3+ls2==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all positions for first bit set to "1", 0..31
+Cover case when rs1=0</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all positions for last bit set to "1", 0..31
+Cover case when rs1=0</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Cover all positions for rs1 to count leading bits, 0..31
+Cover case when rs1=0</t>
+  </si>
+  <si>
+    <t>rD and rs1 should be all possible General Purpose Registers (GPRs).
+Use contrained randm to cover values in range for rs1
+Cover cases when rs1='h0, rs1='hFFFF_FFFF</t>
+  </si>
+  <si>
+    <t>p.ror rD, rs1, rs2</t>
+  </si>
+  <si>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs).
+Cover all extracted bit-widths 0..32
+Cover all bit starting positions 0..31
 Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32</t>
   </si>
   <si>
-    <t>p.extractur instruction</t>
-  </si>
-  <si>
-    <t>p.insert instruction</t>
-  </si>
-  <si>
-    <t>p.insertr instruction</t>
-  </si>
-  <si>
-    <t>p.bclr instruction</t>
-  </si>
-  <si>
-    <t>p.bclrr instruction</t>
-  </si>
-  <si>
-    <t>p.bset instruction</t>
-  </si>
-  <si>
-    <t>p.bsetr instruction</t>
-  </si>
-  <si>
-    <t>p.ff1 instruction</t>
-  </si>
-  <si>
-    <t>p.fl1 instruction</t>
-  </si>
-  <si>
-    <t>p.clb instruction</t>
-  </si>
-  <si>
-    <t>p.cnt instruction</t>
-  </si>
-  <si>
-    <t>p.ror instruction</t>
-  </si>
-  <si>
-    <t>RI5CY: User Manual
-Dec. 2019 Revision 4.2 14.3.1</t>
-  </si>
-  <si>
-    <t>Sub-Feature</t>
-  </si>
-  <si>
-    <t>Feature Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All bit extractions performed as expected.
-</t>
-  </si>
-  <si>
-    <t>Extract ls3 bits from rs1, starting from position ls2.  32-bit sign extend the result.</t>
-  </si>
-  <si>
-    <t>Extract ls3 bits from rs1, starting from position ls2.  32-bit zero extend the result.</t>
-  </si>
-  <si>
-    <t>Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit sign extend the result.</t>
-  </si>
-  <si>
-    <t>Extract rs2[9:5] bits from rs1, starting from position rs2[4:0].  32-bit zero extend the result.</t>
-  </si>
-  <si>
-    <t>Insert rs1[rs2[9:5]] into rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t>Insert rs1[ls3:0] into rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t>Clear ls3 bits in rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t>Clear rs1[rs2[9:5]] bits in rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t>Set ls3 bits in rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t>Set rs1[rs2[9:5]] bits in rD starting from position ls2. No zero or sign extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find first "1" bit in rs1, starting from LSB, and write position in rD.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find last "1" bit in rs1, starting from MSB, and write position in rD.  </t>
-  </si>
-  <si>
-    <t>Count the number of consecutive 1’s or 0’s in rs1 starting from MSB.</t>
-  </si>
-  <si>
-    <t>Count the total number of 1’s in rs1.</t>
-  </si>
-  <si>
-    <t>Rotate right rs1 by rs2 number of bits</t>
-  </si>
-  <si>
-    <t>p.bitrev instruction</t>
-  </si>
-  <si>
-    <t>NEW INSTRUCTION ADDED, NEED CLARIFICATION</t>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs). Cover all extracted bit-widths 0..32
+Cover all bit starting positions 0..31
+ Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32</t>
+  </si>
+  <si>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs). Cover all bit-widths to be inserted 0..32
+Cover all bit starting positions 0..31
+Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32, pass unnaffected bits</t>
+  </si>
+  <si>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs).
+Cover all bit-widths to be cleared 0..32
+Cover all bit starting positions 0..31
+Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32, pass unnaffected bits</t>
+  </si>
+  <si>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs).
+Cover all bit-widths to be set 0..32
+Cover all bit starting positions 0..31
+Cover case when rs2[9:5]+rs2[4:0]==32 and &gt; 32, pass unnaffected bits</t>
+  </si>
+  <si>
+    <t>rD, rs1 and rs2 should be all possible General Purpose Registers (GPRs). Cover all positions for rs1 to count leading bits, 0..31
+Cover cases when rs1='h0, rs1='hFFFF_FFFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Check against ISS</t>
+  </si>
+  <si>
+    <t>OpenHW Compliance, Constrained-Random</t>
+  </si>
+  <si>
+    <t>Functional Coverage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -464,13 +532,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -482,6 +543,20 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -505,8 +580,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFAFF0AF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,10 +594,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -553,12 +629,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D95E0039-98F2-4A40-821A-9D98B3EBA47C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -639,10 +719,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -942,18 +1018,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" customWidth="1"/>
     <col min="5" max="5" width="60.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="35.08984375" style="1" customWidth="1"/>
@@ -964,7 +1039,7 @@
     <col min="1024" max="1025" width="9.08984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -972,10 +1047,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -993,241 +1068,465 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="58">
       <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="58">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="61" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="58">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="58">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="58">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="58">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="72.5">
+      <c r="A9" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="58">
       <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D10" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="72.5">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="58">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="58">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="58">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="58">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="58">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="12" customFormat="1">
+      <c r="A17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="49.5" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:I17"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>